<commit_message>
Atualização do Boletim de Acompanhamento e Relatório Mensal de Pagamentos das OS - Ref. 1ª Quinzena de Out/2016.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201610.xlsx
+++ b/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201610.xlsx
@@ -1710,11 +1710,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3559,10 +3559,10 @@
   <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3860,7 +3860,7 @@
         <v>78</v>
       </c>
       <c r="C5" s="50">
-        <v>42643</v>
+        <v>42647</v>
       </c>
       <c r="D5" t="s">
         <v>96</v>
@@ -3892,8 +3892,8 @@
         <v>148</v>
       </c>
       <c r="O5" s="21">
-        <f>153+OSS[[#This Row],[PF Alterado]]</f>
-        <v>168.5</v>
+        <f>153</f>
+        <v>153</v>
       </c>
       <c r="P5" s="21">
         <v>15.5</v>
@@ -4342,7 +4342,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I51" sqref="I51"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4414,12 +4414,12 @@
       <c r="A3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="26" t="s">
         <v>108</v>
       </c>
@@ -4527,11 +4527,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4721</v>
       </c>
-      <c r="B5" s="114" t="str">
+      <c r="B5" s="113" t="str">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reentregue</v>
       </c>
-      <c r="C5" s="114"/>
+      <c r="C5" s="113"/>
       <c r="D5" s="52" t="str">
         <f>IF(A5="","","em")</f>
         <v>em</v>
@@ -4950,11 +4950,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4757</v>
       </c>
-      <c r="B10" s="114" t="str">
+      <c r="B10" s="113" t="str">
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reentregue</v>
       </c>
-      <c r="C10" s="114"/>
+      <c r="C10" s="113"/>
       <c r="D10" s="52" t="str">
         <f>IF(A10="","","em")</f>
         <v>em</v>
@@ -5373,11 +5373,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4776</v>
       </c>
-      <c r="B15" s="114" t="str">
+      <c r="B15" s="113" t="str">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Recebida_</v>
       </c>
-      <c r="C15" s="114"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="52" t="str">
         <f>IF(A15="","","em")</f>
         <v>em</v>
@@ -5796,18 +5796,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4777</v>
       </c>
-      <c r="B20" s="114" t="str">
+      <c r="B20" s="113" t="str">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reentregue</v>
       </c>
-      <c r="C20" s="114"/>
+      <c r="C20" s="113"/>
       <c r="D20" s="52" t="str">
         <f>IF(A20="","","em")</f>
         <v>em</v>
       </c>
       <c r="E20" s="56">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42643</v>
+        <v>42647</v>
       </c>
       <c r="F20" s="112" t="str">
         <f>IF(A20="","","Titulo:")</f>
@@ -5880,27 +5880,27 @@
       </c>
       <c r="I21" s="20">
         <f>IF(G21="","",G21+ROUND(((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42643</v>
+        <v>42640</v>
       </c>
       <c r="J21" s="20">
         <f>IF(I21="","",WORKDAY(IF(I22="",I21,IF(I22&gt;I21,I22,I21)),IF(IF(P22="",P21,P22)&lt;150,5,10)))</f>
-        <v>42657</v>
+        <v>42654</v>
       </c>
       <c r="K21" s="20">
         <f>IF(J21="","",J21+ROUND((IF(P22="",P21,IF(P22&gt;P21,P22,P21))/(19*LN(IF(P22="",P21,IF(P22&gt;P21,P22,P21)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42676</v>
+        <v>42672</v>
       </c>
       <c r="L21" s="20">
         <f>IF(G21="","",G21+ROUND(((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42682</v>
+        <v>42676</v>
       </c>
       <c r="M21" s="20">
         <f>IF(K21="","",WORKDAY(K21,1))</f>
-        <v>42677</v>
+        <v>42674</v>
       </c>
       <c r="N21" s="20">
         <f>IF(M21="","",M21+SLA_PrazoGarantia)</f>
-        <v>42857</v>
+        <v>42854</v>
       </c>
       <c r="O21" s="27" t="str">
         <f>IF(A20="","","Previsto")</f>
@@ -5912,7 +5912,7 @@
       </c>
       <c r="Q21" s="54">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICP_EOS,1))</f>
-        <v>15.4</v>
+        <v>14.8</v>
       </c>
       <c r="R21" s="21">
         <f>IF(F21="","",SLA_ICP_CIHA)</f>
@@ -5948,7 +5948,7 @@
       </c>
       <c r="Z21" s="54">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICA_EOS,1))</f>
-        <v>38.5</v>
+        <v>37</v>
       </c>
       <c r="AA21" t="str">
         <f>IF(A20="","","Homologação")</f>
@@ -5968,7 +5968,7 @@
       </c>
       <c r="AE21" s="24">
         <f>IF(A20="","",AD21/IF($P22="",$P21,$P22))</f>
-        <v>7.6086956521739135E-2</v>
+        <v>8.3086053412462904E-2</v>
       </c>
       <c r="AF21" s="21">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Atrasos para Correção Homologação",OSS[#Headers],0),FALSE))</f>
@@ -6029,7 +6029,7 @@
         <f>IF(A20="","",IF(VLOOKUP(A20,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A20,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)
 +IF(VLOOKUP(A20,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))
 ))</f>
-        <v>184</v>
+        <v>168.5</v>
       </c>
       <c r="Q22" s="54">
         <f ca="1">IF(F21="","",IF(G22="","",IF(L22="",IF(DataRef&lt;L21,L21,DataRef),L22)-L21))</f>
@@ -6045,11 +6045,11 @@
       </c>
       <c r="T22" s="24">
         <f>IF(J22="","",AB21/IF($P22="",$P21,$P22))</f>
-        <v>5.434782608695652E-2</v>
+        <v>5.9347181008902079E-2</v>
       </c>
       <c r="U22" s="24">
         <f>IF(J22="","",AC21/IF($P22="",$P21,$P22))</f>
-        <v>2.1739130434782608E-2</v>
+        <v>2.3738872403560832E-2</v>
       </c>
       <c r="V22" s="24" t="str">
         <f>IF(K22="","",AB22/IF($P22="",$P21,$P22))</f>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="L23" s="65">
         <f>IF(G21="","",ROUND((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30,0)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="O23" s="27" t="str">
         <f>IF(A20="","","Multa")</f>
@@ -6181,7 +6181,7 @@
       </c>
       <c r="AE23" s="24">
         <f>IF(P21="","",IF(AD23="","",AD23/IF($P22="",$P21,$P22)))</f>
-        <v>7.6086956521739135E-2</v>
+        <v>8.3086053412462904E-2</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
@@ -6195,7 +6195,7 @@
       </c>
       <c r="D24" s="81">
         <f ca="1">IF(P21="","",IF($P22="",$P21,$P22)+IF(D23="",0,D23)-IF(D22="",0,D22))</f>
-        <v>49.199999999999989</v>
+        <v>33.699999999999989</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -6219,11 +6219,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4782</v>
       </c>
-      <c r="B25" s="114" t="str">
+      <c r="B25" s="113" t="str">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Recebida_</v>
       </c>
-      <c r="C25" s="114"/>
+      <c r="C25" s="113"/>
       <c r="D25" s="52" t="str">
         <f>IF(A25="","","em")</f>
         <v>em</v>
@@ -6642,11 +6642,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4797</v>
       </c>
-      <c r="B30" s="114" t="str">
+      <c r="B30" s="113" t="str">
         <f>IF(A30="","",VLOOKUP(A30,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reiniciada</v>
       </c>
-      <c r="C30" s="114"/>
+      <c r="C30" s="113"/>
       <c r="D30" s="52" t="str">
         <f>IF(A30="","","em")</f>
         <v>em</v>
@@ -7065,11 +7065,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4808</v>
       </c>
-      <c r="B35" s="114" t="str">
+      <c r="B35" s="113" t="str">
         <f>IF(A35="","",VLOOKUP(A35,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reiniciada</v>
       </c>
-      <c r="C35" s="114"/>
+      <c r="C35" s="113"/>
       <c r="D35" s="52" t="str">
         <f>IF(A35="","","em")</f>
         <v>em</v>
@@ -7488,11 +7488,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4809</v>
       </c>
-      <c r="B40" s="114" t="str">
+      <c r="B40" s="113" t="str">
         <f>IF(A40="","",VLOOKUP(A40,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Paralisada</v>
       </c>
-      <c r="C40" s="114"/>
+      <c r="C40" s="113"/>
       <c r="D40" s="52" t="str">
         <f>IF(A40="","","em")</f>
         <v>em</v>
@@ -7911,11 +7911,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4810</v>
       </c>
-      <c r="B45" s="114" t="str">
+      <c r="B45" s="113" t="str">
         <f>IF(A45="","",VLOOKUP(A45,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Recebida_</v>
       </c>
-      <c r="C45" s="114"/>
+      <c r="C45" s="113"/>
       <c r="D45" s="52" t="str">
         <f>IF(A45="","","em")</f>
         <v>em</v>
@@ -8334,11 +8334,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4813</v>
       </c>
-      <c r="B50" s="114" t="str">
+      <c r="B50" s="113" t="str">
         <f>IF(A50="","",VLOOKUP(A50,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Plano Entregue</v>
       </c>
-      <c r="C50" s="114"/>
+      <c r="C50" s="113"/>
       <c r="D50" s="52" t="str">
         <f>IF(A50="","","em")</f>
         <v>em</v>
@@ -8757,11 +8757,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B55" s="114" t="str">
+      <c r="B55" s="113" t="str">
         <f>IF(A55="","",VLOOKUP(A55,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C55" s="114"/>
+      <c r="C55" s="113"/>
       <c r="D55" s="52" t="str">
         <f>IF(A55="","","em")</f>
         <v/>
@@ -9180,11 +9180,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B60" s="114" t="str">
+      <c r="B60" s="113" t="str">
         <f>IF(A60="","",VLOOKUP(A60,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C60" s="114"/>
+      <c r="C60" s="113"/>
       <c r="D60" s="52" t="str">
         <f>IF(A60="","","em")</f>
         <v/>
@@ -9603,11 +9603,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B65" s="114" t="str">
+      <c r="B65" s="113" t="str">
         <f>IF(A65="","",VLOOKUP(A65,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C65" s="114"/>
+      <c r="C65" s="113"/>
       <c r="D65" s="52" t="str">
         <f>IF(A65="","","em")</f>
         <v/>
@@ -10026,11 +10026,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B70" s="114" t="str">
+      <c r="B70" s="113" t="str">
         <f>IF(A70="","",VLOOKUP(A70,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C70" s="114"/>
+      <c r="C70" s="113"/>
       <c r="D70" s="52" t="str">
         <f>IF(A70="","","em")</f>
         <v/>
@@ -10449,11 +10449,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B75" s="114" t="str">
+      <c r="B75" s="113" t="str">
         <f>IF(A75="","",VLOOKUP(A75,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C75" s="114"/>
+      <c r="C75" s="113"/>
       <c r="D75" s="52" t="str">
         <f>IF(A75="","","em")</f>
         <v/>
@@ -10872,11 +10872,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B80" s="114" t="str">
+      <c r="B80" s="113" t="str">
         <f>IF(A80="","",VLOOKUP(A80,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C80" s="114"/>
+      <c r="C80" s="113"/>
       <c r="D80" s="52" t="str">
         <f>IF(A80="","","em")</f>
         <v/>
@@ -11295,11 +11295,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B85" s="114" t="str">
+      <c r="B85" s="113" t="str">
         <f>IF(A85="","",VLOOKUP(A85,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C85" s="114"/>
+      <c r="C85" s="113"/>
       <c r="D85" s="52" t="str">
         <f>IF(A85="","","em")</f>
         <v/>
@@ -11718,11 +11718,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B90" s="114" t="str">
+      <c r="B90" s="113" t="str">
         <f>IF(A90="","",VLOOKUP(A90,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C90" s="114"/>
+      <c r="C90" s="113"/>
       <c r="D90" s="52" t="str">
         <f>IF(A90="","","em")</f>
         <v/>
@@ -12141,11 +12141,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B95" s="114" t="str">
+      <c r="B95" s="113" t="str">
         <f>IF(A95="","",VLOOKUP(A95,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C95" s="114"/>
+      <c r="C95" s="113"/>
       <c r="D95" s="52" t="str">
         <f>IF(A95="","","em")</f>
         <v/>
@@ -12564,11 +12564,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B100" s="114" t="str">
+      <c r="B100" s="113" t="str">
         <f>IF(A100="","",VLOOKUP(A100,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C100" s="114"/>
+      <c r="C100" s="113"/>
       <c r="D100" s="52" t="str">
         <f>IF(A100="","","em")</f>
         <v/>
@@ -12987,11 +12987,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B105" s="114" t="str">
+      <c r="B105" s="113" t="str">
         <f>IF(A105="","",VLOOKUP(A105,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C105" s="114"/>
+      <c r="C105" s="113"/>
       <c r="D105" s="52" t="str">
         <f>IF(A105="","","em")</f>
         <v/>
@@ -13410,11 +13410,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B110" s="114" t="str">
+      <c r="B110" s="113" t="str">
         <f>IF(A110="","",VLOOKUP(A110,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C110" s="114"/>
+      <c r="C110" s="113"/>
       <c r="D110" s="52" t="str">
         <f>IF(A110="","","em")</f>
         <v/>
@@ -13833,11 +13833,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B115" s="114" t="str">
+      <c r="B115" s="113" t="str">
         <f>IF(A115="","",VLOOKUP(A115,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C115" s="114"/>
+      <c r="C115" s="113"/>
       <c r="D115" s="52" t="str">
         <f>IF(A115="","","em")</f>
         <v/>
@@ -14256,11 +14256,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B120" s="114" t="str">
+      <c r="B120" s="113" t="str">
         <f>IF(A120="","",VLOOKUP(A120,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C120" s="114"/>
+      <c r="C120" s="113"/>
       <c r="D120" s="52" t="str">
         <f>IF(A120="","","em")</f>
         <v/>
@@ -14679,11 +14679,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B125" s="114" t="str">
+      <c r="B125" s="113" t="str">
         <f>IF(A125="","",VLOOKUP(A125,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C125" s="114"/>
+      <c r="C125" s="113"/>
       <c r="D125" s="52" t="str">
         <f>IF(A125="","","em")</f>
         <v/>
@@ -15102,11 +15102,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B130" s="114" t="str">
+      <c r="B130" s="113" t="str">
         <f>IF(A130="","",VLOOKUP(A130,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C130" s="114"/>
+      <c r="C130" s="113"/>
       <c r="D130" s="52" t="str">
         <f>IF(A130="","","em")</f>
         <v/>
@@ -15525,11 +15525,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B135" s="114" t="str">
+      <c r="B135" s="113" t="str">
         <f>IF(A135="","",VLOOKUP(A135,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C135" s="114"/>
+      <c r="C135" s="113"/>
       <c r="D135" s="52" t="str">
         <f>IF(A135="","","em")</f>
         <v/>
@@ -15948,11 +15948,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B140" s="114" t="str">
+      <c r="B140" s="113" t="str">
         <f>IF(A140="","",VLOOKUP(A140,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C140" s="114"/>
+      <c r="C140" s="113"/>
       <c r="D140" s="52" t="str">
         <f>IF(A140="","","em")</f>
         <v/>
@@ -16371,11 +16371,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B145" s="114" t="str">
+      <c r="B145" s="113" t="str">
         <f>IF(A145="","",VLOOKUP(A145,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C145" s="114"/>
+      <c r="C145" s="113"/>
       <c r="D145" s="52" t="str">
         <f>IF(A145="","","em")</f>
         <v/>
@@ -16794,11 +16794,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B150" s="114" t="str">
+      <c r="B150" s="113" t="str">
         <f>IF(A150="","",VLOOKUP(A150,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C150" s="114"/>
+      <c r="C150" s="113"/>
       <c r="D150" s="52" t="str">
         <f>IF(A150="","","em")</f>
         <v/>
@@ -17214,37 +17214,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B120:C120"/>
     <mergeCell ref="B150:C150"/>
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="B130:C130"/>
     <mergeCell ref="B135:C135"/>
     <mergeCell ref="B140:C140"/>
     <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -19256,7 +19256,7 @@
       </c>
       <c r="F6" s="50">
         <f>IF(C6="","",VLOOKUP(C6,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42643</v>
+        <v>42647</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Atualização do Boletim de Acompanhamento e Relatório Mensal de Pagamentos das OS - Ref. 2ª Quinzena de Out/2016.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201610.xlsx
+++ b/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201610.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Acumulado" sheetId="13" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Mensal!$2:$4</definedName>
     <definedName name="Valor_PF">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="211">
   <si>
     <t>Número OS</t>
   </si>
@@ -699,9 +699,6 @@
   </si>
   <si>
     <t>Do Mês</t>
-  </si>
-  <si>
-    <t>Recebida_</t>
   </si>
   <si>
     <t>Produto ECF - Subproduto Instalador e Atualizador de Versão do Agente Digital Fiscal</t>
@@ -1710,11 +1707,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3562,7 +3559,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,10 +3668,10 @@
         <v>4721</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="C2" s="50">
-        <v>42628</v>
+        <v>42636</v>
       </c>
       <c r="D2" t="s">
         <v>96</v>
@@ -3726,8 +3723,8 @@
       <c r="W2" s="21"/>
       <c r="X2" s="21"/>
       <c r="Y2" s="21">
-        <f>90+15</f>
-        <v>105</v>
+        <f>90+(VALUE("15/10/16")-VALUE("23/09/16")+1)</f>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3735,10 +3732,10 @@
         <v>4757</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="C3" s="50">
-        <v>42639</v>
+        <v>42644</v>
       </c>
       <c r="D3" t="s">
         <v>96</v>
@@ -3760,7 +3757,7 @@
         <v>42500</v>
       </c>
       <c r="K3" s="50">
-        <v>42576</v>
+        <v>42639</v>
       </c>
       <c r="L3" s="50">
         <v>42600</v>
@@ -3788,8 +3785,8 @@
       <c r="W3" s="21"/>
       <c r="X3" s="21"/>
       <c r="Y3" s="21">
-        <f>90+(VALUE("22/09/16")-VALUE("01/09/16")+1)-0</f>
-        <v>112</v>
+        <f>90+(VALUE("22/09/16")-VALUE("01/09/16")+1)+(VALUE("15/10/16")-VALUE("01/10/16")+1)</f>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -3797,10 +3794,10 @@
         <v>4776</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C4" s="50">
-        <v>42628</v>
+        <v>42658</v>
       </c>
       <c r="D4" t="s">
         <v>96</v>
@@ -3848,8 +3845,8 @@
       <c r="W4" s="21"/>
       <c r="X4" s="21"/>
       <c r="Y4" s="21">
-        <f>10+VALUE("17/08/16")-VALUE("18/07/16")+1+(VALUE("07/09/16")-VALUE("11/08/16"))</f>
-        <v>68</v>
+        <f>(VALUE("11/07/16")-VALUE("30/06/16")+1)+(VALUE("17/08/16")-VALUE("18/07/16")+1)+(VALUE("07/09/16")-VALUE("18/08/16")+1)+(VALUE("09/09/16")-VALUE("26/08/16")+1)+(VALUE("15/10/16")-VALUE("16/09/16")+1)</f>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -3857,10 +3854,10 @@
         <v>4777</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="C5" s="50">
-        <v>42647</v>
+        <v>42656</v>
       </c>
       <c r="D5" t="s">
         <v>96</v>
@@ -3882,7 +3879,7 @@
         <v>42528</v>
       </c>
       <c r="K5" s="50">
-        <v>42607</v>
+        <v>42647</v>
       </c>
       <c r="L5" s="50">
         <v>42628</v>
@@ -3902,7 +3899,7 @@
         <v>134.80000000000001</v>
       </c>
       <c r="R5" s="21">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S5" s="21">
         <v>4</v>
@@ -3913,8 +3910,8 @@
       <c r="W5" s="21"/>
       <c r="X5" s="21"/>
       <c r="Y5" s="21">
-        <f>VALUE("09/08/16")-VALUE("20/07/16")+1+(VALUE("27/09/16")-VALUE("22/08/16"))</f>
-        <v>57</v>
+        <f>(VALUE("09/08/16")-VALUE("20/07/16")+1)+(VALUE("27/09/16")-VALUE("22/08/16")+1)+(VALUE("15/10/16")-VALUE("04/10/16")+1)</f>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -3922,10 +3919,10 @@
         <v>4782</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>78</v>
       </c>
       <c r="C6" s="50">
-        <v>42628</v>
+        <v>42660</v>
       </c>
       <c r="D6" t="s">
         <v>96</v>
@@ -3947,7 +3944,7 @@
         <v>42543</v>
       </c>
       <c r="K6" s="50">
-        <v>42622</v>
+        <v>42660</v>
       </c>
       <c r="L6" s="50">
         <v>42628</v>
@@ -3963,16 +3960,20 @@
       <c r="Q6" s="66">
         <v>128</v>
       </c>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
+      <c r="R6" s="21">
+        <v>8</v>
+      </c>
+      <c r="S6" s="21">
+        <v>4</v>
+      </c>
       <c r="T6" s="21"/>
       <c r="U6" s="21"/>
       <c r="V6" s="21"/>
       <c r="W6" s="21"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="21">
-        <f>VALUE("19/08/16")-VALUE("04/08/16")+1</f>
-        <v>16</v>
+        <f>(VALUE("19/08/16")-VALUE("04/08/16")+1)+(VALUE("13/10/16")-VALUE("15/09/16")+1)</f>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -4010,8 +4011,12 @@
       <c r="N7" s="21">
         <v>50</v>
       </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
+      <c r="O7" s="21">
+        <v>53</v>
+      </c>
+      <c r="P7" s="21">
+        <v>17</v>
+      </c>
       <c r="Q7" s="66"/>
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
@@ -4021,8 +4026,8 @@
       <c r="W7" s="21"/>
       <c r="X7" s="21"/>
       <c r="Y7" s="21">
-        <f>(VALUE("08/08/16")-VALUE("18/07/16")+1)+(VALUE("04/10/16")-VALUE("16/08/16")+1)</f>
-        <v>72</v>
+        <f>(VALUE("08/08/16")-VALUE("18/07/16")+1)+(VALUE("04/10/16")-VALUE("16/08/16")+1)+(VALUE("13/10/16")-VALUE("16/09/16")+1)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -4119,8 +4124,8 @@
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
       <c r="Y9" s="21">
-        <f>(VALUE("04/10/16")-VALUE("22/08/16")+1)</f>
-        <v>44</v>
+        <f>(VALUE("15/10/16")-VALUE("22/08/16")+1)</f>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -4128,10 +4133,10 @@
         <v>4810</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>145</v>
       </c>
       <c r="C10" s="50">
-        <v>42639</v>
+        <v>42646</v>
       </c>
       <c r="D10" t="s">
         <v>96</v>
@@ -4179,8 +4184,8 @@
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
       <c r="Y10" s="21">
-        <f>(VALUE("06/09/16")-VALUE("26/08/16")+1)+15</f>
-        <v>27</v>
+        <f>(VALUE("06/09/16")-VALUE("26/08/16")+1)+(VALUE("15/10/16")-VALUE("27/09/16")+1)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -4191,7 +4196,7 @@
         <v>136</v>
       </c>
       <c r="C11" s="50">
-        <v>42633</v>
+        <v>42647</v>
       </c>
       <c r="D11" t="s">
         <v>96</v>
@@ -4200,7 +4205,7 @@
         <v>187</v>
       </c>
       <c r="F11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G11" s="50">
         <v>42633</v>
@@ -4338,11 +4343,11 @@
   </sheetPr>
   <dimension ref="A1:AG154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,7 +4378,7 @@
         <v>119</v>
       </c>
       <c r="B1" s="61">
-        <v>42648</v>
+        <v>42658</v>
       </c>
       <c r="D1" s="59"/>
       <c r="E1" s="62" t="s">
@@ -4414,12 +4419,12 @@
       <c r="A3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
       <c r="F3" s="26" t="s">
         <v>108</v>
       </c>
@@ -4527,18 +4532,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4721</v>
       </c>
-      <c r="B5" s="113" t="str">
+      <c r="B5" s="114" t="str">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Reentregue</v>
-      </c>
-      <c r="C5" s="113"/>
+        <v>Paralisada</v>
+      </c>
+      <c r="C5" s="114"/>
       <c r="D5" s="52" t="str">
         <f>IF(A5="","","em")</f>
         <v>em</v>
       </c>
       <c r="E5" s="56">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42628</v>
+        <v>42636</v>
       </c>
       <c r="F5" s="111" t="str">
         <f>IF(A5="","","Titulo:")</f>
@@ -4611,27 +4616,27 @@
       </c>
       <c r="I6" s="20">
         <f>IF(G6="","",G6+ROUND(((IF(P7="",P6,P7)/(19*LN(IF(P7="",P6,P7))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42620</v>
+        <v>42628</v>
       </c>
       <c r="J6" s="20">
         <f>IF(I6="","",WORKDAY(IF(I7="",I6,IF(I7&gt;I6,I7,I6)),IF(IF(P7="",P6,P7)&lt;150,5,10)))</f>
-        <v>42634</v>
+        <v>42642</v>
       </c>
       <c r="K6" s="20">
         <f>IF(J6="","",J6+ROUND((IF(P7="",P6,IF(P7&gt;P6,P7,P6))/(19*LN(IF(P7="",P6,IF(P7&gt;P6,P7,P6)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42659</v>
+        <v>42667</v>
       </c>
       <c r="L6" s="20">
         <f>IF(G6="","",G6+ROUND(((IF(P7="",P6,P7)/(19*LN(IF(P7="",P6,P7))-42))*30)+IF(VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42670</v>
+        <v>42678</v>
       </c>
       <c r="M6" s="20">
         <f>IF(K6="","",WORKDAY(K6,1))</f>
-        <v>42660</v>
+        <v>42668</v>
       </c>
       <c r="N6" s="20">
         <f>IF(M6="","",M6+SLA_PrazoGarantia)</f>
-        <v>42840</v>
+        <v>42848</v>
       </c>
       <c r="O6" s="27" t="str">
         <f>IF(A5="","","Previsto")</f>
@@ -4643,7 +4648,7 @@
       </c>
       <c r="Q6" s="54">
         <f>IF(F6="","",ROUND((L6-G6)*SLA_ICP_EOS,1))</f>
-        <v>23.1</v>
+        <v>23.9</v>
       </c>
       <c r="R6" s="21">
         <f>IF(F6="","",SLA_ICP_CIHA)</f>
@@ -4679,7 +4684,7 @@
       </c>
       <c r="Z6" s="54">
         <f>IF(F6="","",ROUND((L6-G6)*SLA_ICA_EOS,1))</f>
-        <v>57.8</v>
+        <v>59.8</v>
       </c>
       <c r="AA6" t="str">
         <f>IF(A5="","","Homologação")</f>
@@ -4844,7 +4849,7 @@
       </c>
       <c r="L8" s="65">
         <f>IF(G6="","",ROUND((IF(P7="",P6,P7)/(19*LN(IF(P7="",P6,P7))-42))*30,0)+IF(VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="O8" s="27" t="str">
         <f>IF(A5="","","Multa")</f>
@@ -4938,7 +4943,7 @@
       </c>
       <c r="L9" s="65">
         <f>IF(G6="","",IF(IFERROR(VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A5,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
@@ -4950,18 +4955,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4757</v>
       </c>
-      <c r="B10" s="113" t="str">
+      <c r="B10" s="114" t="str">
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Reentregue</v>
-      </c>
-      <c r="C10" s="113"/>
+        <v>Paralisada</v>
+      </c>
+      <c r="C10" s="114"/>
       <c r="D10" s="52" t="str">
         <f>IF(A10="","","em")</f>
         <v>em</v>
       </c>
       <c r="E10" s="56">
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42639</v>
+        <v>42644</v>
       </c>
       <c r="F10" s="112" t="str">
         <f>IF(A10="","","Titulo:")</f>
@@ -5034,27 +5039,27 @@
       </c>
       <c r="I11" s="20">
         <f>IF(G11="","",G11+ROUND(((IF(P12="",P11,P12)/(19*LN(IF(P12="",P11,P12))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42643</v>
+        <v>42658</v>
       </c>
       <c r="J11" s="20">
         <f>IF(I11="","",WORKDAY(IF(I12="",I11,IF(I12&gt;I11,I12,I11)),IF(IF(P12="",P11,P12)&lt;150,5,10)))</f>
-        <v>42650</v>
+        <v>42664</v>
       </c>
       <c r="K11" s="20">
         <f>IF(J11="","",J11+ROUND((IF(P12="",P11,IF(P12&gt;P11,P12,P11))/(19*LN(IF(P12="",P11,IF(P12&gt;P11,P12,P11)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42663</v>
+        <v>42677</v>
       </c>
       <c r="L11" s="20">
         <f>IF(G11="","",G11+ROUND(((IF(P12="",P11,P12)/(19*LN(IF(P12="",P11,P12))-42))*30)+IF(VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42669</v>
+        <v>42684</v>
       </c>
       <c r="M11" s="20">
         <f>IF(K11="","",WORKDAY(K11,1))</f>
-        <v>42664</v>
+        <v>42678</v>
       </c>
       <c r="N11" s="20">
         <f>IF(M11="","",M11+SLA_PrazoGarantia)</f>
-        <v>42844</v>
+        <v>42858</v>
       </c>
       <c r="O11" s="27" t="str">
         <f>IF(A10="","","Previsto")</f>
@@ -5066,7 +5071,7 @@
       </c>
       <c r="Q11" s="54">
         <f>IF(F11="","",ROUND((L11-G11)*SLA_ICP_EOS,1))</f>
-        <v>17.600000000000001</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="R11" s="21">
         <f>IF(F11="","",SLA_ICP_CIHA)</f>
@@ -5102,7 +5107,7 @@
       </c>
       <c r="Z11" s="54">
         <f>IF(F11="","",ROUND((L11-G11)*SLA_ICA_EOS,1))</f>
-        <v>44</v>
+        <v>47.8</v>
       </c>
       <c r="AA11" t="str">
         <f>IF(A10="","","Homologação")</f>
@@ -5153,7 +5158,7 @@
       </c>
       <c r="I12" s="20">
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
-        <v>42576</v>
+        <v>42639</v>
       </c>
       <c r="J12" s="20">
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)))</f>
@@ -5267,7 +5272,7 @@
       </c>
       <c r="L13" s="65">
         <f>IF(G11="","",ROUND((IF(P12="",P11,P12)/(19*LN(IF(P12="",P11,P12))-42))*30,0)+IF(VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="O13" s="27" t="str">
         <f>IF(A10="","","Multa")</f>
@@ -5361,7 +5366,7 @@
       </c>
       <c r="L14" s="65">
         <f>IF(G11="","",IF(IFERROR(VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A10,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
@@ -5373,18 +5378,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4776</v>
       </c>
-      <c r="B15" s="113" t="str">
+      <c r="B15" s="114" t="str">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Recebida_</v>
-      </c>
-      <c r="C15" s="113"/>
+        <v>Reiniciada</v>
+      </c>
+      <c r="C15" s="114"/>
       <c r="D15" s="52" t="str">
         <f>IF(A15="","","em")</f>
         <v>em</v>
       </c>
       <c r="E15" s="56">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42628</v>
+        <v>42658</v>
       </c>
       <c r="F15" s="112" t="str">
         <f>IF(A15="","","Titulo:")</f>
@@ -5457,27 +5462,27 @@
       </c>
       <c r="I16" s="20">
         <f>IF(G16="","",G16+ROUND(((IF(P17="",P16,P17)/(19*LN(IF(P17="",P16,P17))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42630</v>
+        <v>42671</v>
       </c>
       <c r="J16" s="20">
         <f>IF(I16="","",WORKDAY(IF(I17="",I16,IF(I17&gt;I16,I17,I16)),IF(IF(P17="",P16,P17)&lt;150,5,10)))</f>
-        <v>42636</v>
+        <v>42678</v>
       </c>
       <c r="K16" s="20">
         <f>IF(J16="","",J16+ROUND((IF(P17="",P16,IF(P17&gt;P16,P17,P16))/(19*LN(IF(P17="",P16,IF(P17&gt;P16,P17,P16)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42650</v>
+        <v>42692</v>
       </c>
       <c r="L16" s="20">
         <f>IF(G16="","",G16+ROUND(((IF(P17="",P16,P17)/(19*LN(IF(P17="",P16,P17))-42))*30)+IF(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42658</v>
+        <v>42699</v>
       </c>
       <c r="M16" s="20">
         <f>IF(K16="","",WORKDAY(K16,1))</f>
-        <v>42653</v>
+        <v>42695</v>
       </c>
       <c r="N16" s="20">
         <f>IF(M16="","",M16+SLA_PrazoGarantia)</f>
-        <v>42833</v>
+        <v>42875</v>
       </c>
       <c r="O16" s="27" t="str">
         <f>IF(A15="","","Previsto")</f>
@@ -5489,7 +5494,7 @@
       </c>
       <c r="Q16" s="54">
         <f>IF(F16="","",ROUND((L16-G16)*SLA_ICP_EOS,1))</f>
-        <v>13.7</v>
+        <v>17.8</v>
       </c>
       <c r="R16" s="21">
         <f>IF(F16="","",SLA_ICP_CIHA)</f>
@@ -5525,7 +5530,7 @@
       </c>
       <c r="Z16" s="54">
         <f>IF(F16="","",ROUND((L16-G16)*SLA_ICA_EOS,1))</f>
-        <v>34.299999999999997</v>
+        <v>44.5</v>
       </c>
       <c r="AA16" t="str">
         <f>IF(A15="","","Homologação")</f>
@@ -5690,7 +5695,7 @@
       </c>
       <c r="L18" s="65">
         <f>IF(G16="","",ROUND((IF(P17="",P16,P17)/(19*LN(IF(P17="",P16,P17))-42))*30,0)+IF(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="O18" s="27" t="str">
         <f>IF(A15="","","Multa")</f>
@@ -5784,7 +5789,7 @@
       </c>
       <c r="L19" s="65">
         <f>IF(G16="","",IF(IFERROR(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="M19" s="20"/>
       <c r="N19" s="20"/>
@@ -5796,18 +5801,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4777</v>
       </c>
-      <c r="B20" s="113" t="str">
+      <c r="B20" s="114" t="str">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Reentregue</v>
-      </c>
-      <c r="C20" s="113"/>
+        <v>Paralisada</v>
+      </c>
+      <c r="C20" s="114"/>
       <c r="D20" s="52" t="str">
         <f>IF(A20="","","em")</f>
         <v>em</v>
       </c>
       <c r="E20" s="56">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42647</v>
+        <v>42656</v>
       </c>
       <c r="F20" s="112" t="str">
         <f>IF(A20="","","Titulo:")</f>
@@ -5880,27 +5885,27 @@
       </c>
       <c r="I21" s="20">
         <f>IF(G21="","",G21+ROUND(((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42640</v>
+        <v>42653</v>
       </c>
       <c r="J21" s="20">
         <f>IF(I21="","",WORKDAY(IF(I22="",I21,IF(I22&gt;I21,I22,I21)),IF(IF(P22="",P21,P22)&lt;150,5,10)))</f>
-        <v>42654</v>
+        <v>42667</v>
       </c>
       <c r="K21" s="20">
         <f>IF(J21="","",J21+ROUND((IF(P22="",P21,IF(P22&gt;P21,P22,P21))/(19*LN(IF(P22="",P21,IF(P22&gt;P21,P22,P21)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42672</v>
+        <v>42685</v>
       </c>
       <c r="L21" s="20">
         <f>IF(G21="","",G21+ROUND(((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42676</v>
+        <v>42689</v>
       </c>
       <c r="M21" s="20">
         <f>IF(K21="","",WORKDAY(K21,1))</f>
-        <v>42674</v>
+        <v>42688</v>
       </c>
       <c r="N21" s="20">
         <f>IF(M21="","",M21+SLA_PrazoGarantia)</f>
-        <v>42854</v>
+        <v>42868</v>
       </c>
       <c r="O21" s="27" t="str">
         <f>IF(A20="","","Previsto")</f>
@@ -5912,7 +5917,7 @@
       </c>
       <c r="Q21" s="54">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICP_EOS,1))</f>
-        <v>14.8</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="R21" s="21">
         <f>IF(F21="","",SLA_ICP_CIHA)</f>
@@ -5948,7 +5953,7 @@
       </c>
       <c r="Z21" s="54">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICA_EOS,1))</f>
-        <v>37</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="AA21" t="str">
         <f>IF(A20="","","Homologação")</f>
@@ -5956,7 +5961,7 @@
       </c>
       <c r="AB21" s="21">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Não Grave - Homologação",OSS[#Headers],0),FALSE))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AC21" s="21">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Grave - Homologação",OSS[#Headers],0),FALSE))</f>
@@ -5964,11 +5969,11 @@
       </c>
       <c r="AD21" s="21">
         <f>IF(A20="","",AB21+AC21)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AE21" s="24">
         <f>IF(A20="","",AD21/IF($P22="",$P21,$P22))</f>
-        <v>8.3086053412462904E-2</v>
+        <v>7.1216617210682495E-2</v>
       </c>
       <c r="AF21" s="21">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Atrasos para Correção Homologação",OSS[#Headers],0),FALSE))</f>
@@ -5999,7 +6004,7 @@
       </c>
       <c r="I22" s="20">
         <f>IF(A20="","",IF(VLOOKUP(A20,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A20,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
-        <v>42607</v>
+        <v>42647</v>
       </c>
       <c r="J22" s="20">
         <f>IF(A20="","",IF(VLOOKUP(A20,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A20,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)))</f>
@@ -6045,7 +6050,7 @@
       </c>
       <c r="T22" s="24">
         <f>IF(J22="","",AB21/IF($P22="",$P21,$P22))</f>
-        <v>5.9347181008902079E-2</v>
+        <v>4.7477744807121663E-2</v>
       </c>
       <c r="U22" s="24">
         <f>IF(J22="","",AC21/IF($P22="",$P21,$P22))</f>
@@ -6113,7 +6118,7 @@
       </c>
       <c r="L23" s="65">
         <f>IF(G21="","",ROUND((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30,0)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="O23" s="27" t="str">
         <f>IF(A20="","","Multa")</f>
@@ -6169,7 +6174,7 @@
       </c>
       <c r="AB23" s="21">
         <f>IF(SUM(AB21:AB22)=0,"",SUM(AB21:AB22))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AC23" s="21">
         <f>IF(SUM(AC21:AC22)=0,"",SUM(AC21:AC22))</f>
@@ -6177,11 +6182,11 @@
       </c>
       <c r="AD23" s="21">
         <f>IF(SUM(AB23:AC23)=0,"",SUM(AB23:AC23))</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AE23" s="24">
         <f>IF(P21="","",IF(AD23="","",AD23/IF($P22="",$P21,$P22)))</f>
-        <v>8.3086053412462904E-2</v>
+        <v>7.1216617210682495E-2</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
@@ -6207,7 +6212,7 @@
       </c>
       <c r="L24" s="65">
         <f>IF(G21="","",IF(IFERROR(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="M24" s="20"/>
       <c r="N24" s="20"/>
@@ -6219,18 +6224,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4782</v>
       </c>
-      <c r="B25" s="113" t="str">
+      <c r="B25" s="114" t="str">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Recebida_</v>
-      </c>
-      <c r="C25" s="113"/>
+        <v>Reentregue</v>
+      </c>
+      <c r="C25" s="114"/>
       <c r="D25" s="52" t="str">
         <f>IF(A25="","","em")</f>
         <v>em</v>
       </c>
       <c r="E25" s="56">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42628</v>
+        <v>42660</v>
       </c>
       <c r="F25" s="112" t="str">
         <f>IF(A25="","","Titulo:")</f>
@@ -6303,27 +6308,27 @@
       </c>
       <c r="I26" s="20">
         <f>IF(G26="","",G26+ROUND(((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42605</v>
+        <v>42634</v>
       </c>
       <c r="J26" s="20">
         <f>IF(I26="","",WORKDAY(IF(I27="",I26,IF(I27&gt;I26,I27,I26)),IF(IF(P27="",P26,P27)&lt;150,5,10)))</f>
-        <v>42636</v>
+        <v>42674</v>
       </c>
       <c r="K26" s="20">
         <f>IF(J26="","",J26+ROUND((IF(P27="",P26,IF(P27&gt;P26,P27,P26))/(19*LN(IF(P27="",P26,IF(P27&gt;P26,P27,P26)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42654</v>
+        <v>42692</v>
       </c>
       <c r="L26" s="20">
         <f>IF(G26="","",G26+ROUND(((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30)+IF(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42640</v>
+        <v>42669</v>
       </c>
       <c r="M26" s="20">
         <f>IF(K26="","",WORKDAY(K26,1))</f>
-        <v>42655</v>
+        <v>42695</v>
       </c>
       <c r="N26" s="20">
         <f>IF(M26="","",M26+SLA_PrazoGarantia)</f>
-        <v>42835</v>
+        <v>42875</v>
       </c>
       <c r="O26" s="27" t="str">
         <f>IF(A25="","","Previsto")</f>
@@ -6335,7 +6340,7 @@
       </c>
       <c r="Q26" s="54">
         <f>IF(F26="","",ROUND((L26-G26)*SLA_ICP_EOS,1))</f>
-        <v>10.4</v>
+        <v>13.3</v>
       </c>
       <c r="R26" s="21">
         <f>IF(F26="","",SLA_ICP_CIHA)</f>
@@ -6371,7 +6376,7 @@
       </c>
       <c r="Z26" s="54">
         <f>IF(F26="","",ROUND((L26-G26)*SLA_ICA_EOS,1))</f>
-        <v>26</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="AA26" t="str">
         <f>IF(A25="","","Homologação")</f>
@@ -6379,19 +6384,19 @@
       </c>
       <c r="AB26" s="21">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Não Grave - Homologação",OSS[#Headers],0),FALSE))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC26" s="21">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Grave - Homologação",OSS[#Headers],0),FALSE))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD26" s="21">
         <f>IF(A25="","",AB26+AC26)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AE26" s="24">
         <f>IF(A25="","",AD26/IF($P27="",$P26,$P27))</f>
-        <v>0</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="AF26" s="21">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Atrasos para Correção Homologação",OSS[#Headers],0),FALSE))</f>
@@ -6422,7 +6427,7 @@
       </c>
       <c r="I27" s="20">
         <f>IF(A25="","",IF(VLOOKUP(A25,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A25,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
-        <v>42622</v>
+        <v>42660</v>
       </c>
       <c r="J27" s="20">
         <f>IF(A25="","",IF(VLOOKUP(A25,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A25,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)))</f>
@@ -6456,7 +6461,7 @@
       </c>
       <c r="Q27" s="54">
         <f ca="1">IF(F26="","",IF(G27="","",IF(L27="",IF(DataRef&lt;L26,L26,DataRef),L27)-L26))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R27" s="21">
         <f>IF(J27="","",AF26)</f>
@@ -6468,11 +6473,11 @@
       </c>
       <c r="T27" s="24">
         <f>IF(J27="","",AB26/IF($P27="",$P26,$P27))</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="U27" s="24">
         <f>IF(J27="","",AC26/IF($P27="",$P26,$P27))</f>
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="V27" s="24" t="str">
         <f>IF(K27="","",AB27/IF($P27="",$P26,$P27))</f>
@@ -6492,7 +6497,7 @@
       </c>
       <c r="Z27" s="54">
         <f ca="1">IF(F26="","",IF(L27="",IF(DataRef&lt;L26,L26,DataRef),L27)-L26)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AA27" t="str">
         <f>IF(A25="","","Garantia")</f>
@@ -6536,7 +6541,7 @@
       </c>
       <c r="L28" s="65">
         <f>IF(G26="","",ROUND((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30,0)+IF(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="O28" s="27" t="str">
         <f>IF(A25="","","Multa")</f>
@@ -6590,21 +6595,21 @@
         <f>IF(A25="","","Total")</f>
         <v>Total</v>
       </c>
-      <c r="AB28" s="21" t="str">
+      <c r="AB28" s="21">
         <f>IF(SUM(AB26:AB27)=0,"",SUM(AB26:AB27))</f>
-        <v/>
-      </c>
-      <c r="AC28" s="21" t="str">
+        <v>8</v>
+      </c>
+      <c r="AC28" s="21">
         <f>IF(SUM(AC26:AC27)=0,"",SUM(AC26:AC27))</f>
-        <v/>
-      </c>
-      <c r="AD28" s="21" t="str">
+        <v>4</v>
+      </c>
+      <c r="AD28" s="21">
         <f>IF(SUM(AB28:AC28)=0,"",SUM(AB28:AC28))</f>
-        <v/>
-      </c>
-      <c r="AE28" s="24" t="str">
+        <v>12</v>
+      </c>
+      <c r="AE28" s="24">
         <f>IF(P26="","",IF(AD28="","",AD28/IF($P27="",$P26,$P27)))</f>
-        <v/>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="29" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
@@ -6630,7 +6635,7 @@
       </c>
       <c r="L29" s="65">
         <f>IF(G26="","",IF(IFERROR(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="M29" s="20"/>
       <c r="N29" s="20"/>
@@ -6642,11 +6647,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4797</v>
       </c>
-      <c r="B30" s="113" t="str">
+      <c r="B30" s="114" t="str">
         <f>IF(A30="","",VLOOKUP(A30,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reiniciada</v>
       </c>
-      <c r="C30" s="113"/>
+      <c r="C30" s="114"/>
       <c r="D30" s="52" t="str">
         <f>IF(A30="","","em")</f>
         <v>em</v>
@@ -6726,27 +6731,27 @@
       </c>
       <c r="I31" s="20">
         <f>IF(G31="","",G31+ROUND(((IF(P32="",P31,P32)/(19*LN(IF(P32="",P31,P32))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42657</v>
+        <v>42690</v>
       </c>
       <c r="J31" s="20">
         <f>IF(I31="","",WORKDAY(IF(I32="",I31,IF(I32&gt;I31,I32,I31)),IF(IF(P32="",P31,P32)&lt;150,5,10)))</f>
-        <v>42664</v>
+        <v>42697</v>
       </c>
       <c r="K31" s="20">
         <f>IF(J31="","",J31+ROUND((IF(P32="",P31,IF(P32&gt;P31,P32,P31))/(19*LN(IF(P32="",P31,IF(P32&gt;P31,P32,P31)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42673</v>
+        <v>42708</v>
       </c>
       <c r="L31" s="20">
         <f>IF(G31="","",G31+ROUND(((IF(P32="",P31,P32)/(19*LN(IF(P32="",P31,P32))-42))*30)+IF(VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42675</v>
+        <v>42711</v>
       </c>
       <c r="M31" s="20">
         <f>IF(K31="","",WORKDAY(K31,1))</f>
-        <v>42674</v>
+        <v>42709</v>
       </c>
       <c r="N31" s="20">
         <f>IF(M31="","",M31+SLA_PrazoGarantia)</f>
-        <v>42854</v>
+        <v>42889</v>
       </c>
       <c r="O31" s="27" t="str">
         <f>IF(A30="","","Previsto")</f>
@@ -6758,7 +6763,7 @@
       </c>
       <c r="Q31" s="54">
         <f>IF(F31="","",ROUND((L31-G31)*SLA_ICP_EOS,1))</f>
-        <v>11.8</v>
+        <v>15.4</v>
       </c>
       <c r="R31" s="21">
         <f>IF(F31="","",SLA_ICP_CIHA)</f>
@@ -6794,7 +6799,7 @@
       </c>
       <c r="Z31" s="54">
         <f>IF(F31="","",ROUND((L31-G31)*SLA_ICA_EOS,1))</f>
-        <v>29.5</v>
+        <v>38.5</v>
       </c>
       <c r="AA31" t="str">
         <f>IF(A30="","","Homologação")</f>
@@ -6871,11 +6876,11 @@
         <f>IF(A30="","","Apurado")</f>
         <v>Apurado</v>
       </c>
-      <c r="P32" s="21" t="str">
+      <c r="P32" s="21">
         <f>IF(A30="","",IF(VLOOKUP(A30,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A30,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)
 +IF(VLOOKUP(A30,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A30,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))
 ))</f>
-        <v/>
+        <v>70</v>
       </c>
       <c r="Q32" s="54">
         <f ca="1">IF(F31="","",IF(G32="","",IF(L32="",IF(DataRef&lt;L31,L31,DataRef),L32)-L31))</f>
@@ -6959,7 +6964,7 @@
       </c>
       <c r="L33" s="65">
         <f>IF(G31="","",ROUND((IF(P32="",P31,P32)/(19*LN(IF(P32="",P31,P32))-42))*30,0)+IF(VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="O33" s="27" t="str">
         <f>IF(A30="","","Multa")</f>
@@ -7041,7 +7046,7 @@
       </c>
       <c r="D34" s="81">
         <f ca="1">IF(P31="","",IF($P32="",$P31,$P32)+IF(D33="",0,D33)-IF(D32="",0,D32))</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -7053,7 +7058,7 @@
       </c>
       <c r="L34" s="65">
         <f>IF(G31="","",IF(IFERROR(VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A30,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="M34" s="20"/>
       <c r="N34" s="20"/>
@@ -7065,11 +7070,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4808</v>
       </c>
-      <c r="B35" s="113" t="str">
+      <c r="B35" s="114" t="str">
         <f>IF(A35="","",VLOOKUP(A35,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reiniciada</v>
       </c>
-      <c r="C35" s="113"/>
+      <c r="C35" s="114"/>
       <c r="D35" s="52" t="str">
         <f>IF(A35="","","em")</f>
         <v>em</v>
@@ -7488,11 +7493,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4809</v>
       </c>
-      <c r="B40" s="113" t="str">
+      <c r="B40" s="114" t="str">
         <f>IF(A40="","",VLOOKUP(A40,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Paralisada</v>
       </c>
-      <c r="C40" s="113"/>
+      <c r="C40" s="114"/>
       <c r="D40" s="52" t="str">
         <f>IF(A40="","","em")</f>
         <v>em</v>
@@ -7572,27 +7577,27 @@
       </c>
       <c r="I41" s="20">
         <f>IF(G41="","",G41+ROUND(((IF(P42="",P41,P42)/(19*LN(IF(P42="",P41,P42))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42715</v>
+        <v>42726</v>
       </c>
       <c r="J41" s="20">
         <f>IF(I41="","",WORKDAY(IF(I42="",I41,IF(I42&gt;I41,I42,I41)),IF(IF(P42="",P41,P42)&lt;150,5,10)))</f>
-        <v>42727</v>
+        <v>42740</v>
       </c>
       <c r="K41" s="20">
         <f>IF(J41="","",J41+ROUND((IF(P42="",P41,IF(P42&gt;P41,P42,P41))/(19*LN(IF(P42="",P41,IF(P42&gt;P41,P42,P41)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42749</v>
+        <v>42762</v>
       </c>
       <c r="L41" s="20">
         <f>IF(G41="","",G41+ROUND(((IF(P42="",P41,P42)/(19*LN(IF(P42="",P41,P42))-42))*30)+IF(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42759</v>
+        <v>42770</v>
       </c>
       <c r="M41" s="20">
         <f>IF(K41="","",WORKDAY(K41,1))</f>
-        <v>42751</v>
+        <v>42765</v>
       </c>
       <c r="N41" s="20">
         <f>IF(M41="","",M41+SLA_PrazoGarantia)</f>
-        <v>42931</v>
+        <v>42945</v>
       </c>
       <c r="O41" s="27" t="str">
         <f>IF(A40="","","Previsto")</f>
@@ -7604,7 +7609,7 @@
       </c>
       <c r="Q41" s="54">
         <f>IF(F41="","",ROUND((L41-G41)*SLA_ICP_EOS,1))</f>
-        <v>15.4</v>
+        <v>16.5</v>
       </c>
       <c r="R41" s="21">
         <f>IF(F41="","",SLA_ICP_CIHA)</f>
@@ -7640,7 +7645,7 @@
       </c>
       <c r="Z41" s="54">
         <f>IF(F41="","",ROUND((L41-G41)*SLA_ICA_EOS,1))</f>
-        <v>38.5</v>
+        <v>41.3</v>
       </c>
       <c r="AA41" t="str">
         <f>IF(A40="","","Homologação")</f>
@@ -7805,7 +7810,7 @@
       </c>
       <c r="L43" s="65">
         <f>IF(G41="","",ROUND((IF(P42="",P41,P42)/(19*LN(IF(P42="",P41,P42))-42))*30,0)+IF(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="O43" s="27" t="str">
         <f>IF(A40="","","Multa")</f>
@@ -7899,7 +7904,7 @@
       </c>
       <c r="L44" s="65">
         <f>IF(G41="","",IF(IFERROR(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
@@ -7911,18 +7916,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4810</v>
       </c>
-      <c r="B45" s="113" t="str">
+      <c r="B45" s="114" t="str">
         <f>IF(A45="","",VLOOKUP(A45,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Recebida_</v>
-      </c>
-      <c r="C45" s="113"/>
+        <v>Paralisada</v>
+      </c>
+      <c r="C45" s="114"/>
       <c r="D45" s="52" t="str">
         <f>IF(A45="","","em")</f>
         <v>em</v>
       </c>
       <c r="E45" s="56">
         <f>IF(A45="","",VLOOKUP(A45,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42639</v>
+        <v>42646</v>
       </c>
       <c r="F45" s="112" t="str">
         <f>IF(A45="","","Titulo:")</f>
@@ -7995,27 +8000,27 @@
       </c>
       <c r="I46" s="20">
         <f>IF(G46="","",G46+ROUND(((IF(P47="",P46,P47)/(19*LN(IF(P47="",P46,P47))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42648</v>
+        <v>42652</v>
       </c>
       <c r="J46" s="20">
         <f>IF(I46="","",WORKDAY(IF(I47="",I46,IF(I47&gt;I46,I47,I46)),IF(IF(P47="",P46,P47)&lt;150,5,10)))</f>
-        <v>42655</v>
+        <v>42657</v>
       </c>
       <c r="K46" s="20">
         <f>IF(J46="","",J46+ROUND((IF(P47="",P46,IF(P47&gt;P46,P47,P46))/(19*LN(IF(P47="",P46,IF(P47&gt;P46,P47,P46)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42663</v>
+        <v>42665</v>
       </c>
       <c r="L46" s="20">
         <f>IF(G46="","",G46+ROUND(((IF(P47="",P46,P47)/(19*LN(IF(P47="",P46,P47))-42))*30)+IF(VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42664</v>
+        <v>42668</v>
       </c>
       <c r="M46" s="20">
         <f>IF(K46="","",WORKDAY(K46,1))</f>
-        <v>42664</v>
+        <v>42667</v>
       </c>
       <c r="N46" s="20">
         <f>IF(M46="","",M46+SLA_PrazoGarantia)</f>
-        <v>42844</v>
+        <v>42847</v>
       </c>
       <c r="O46" s="27" t="str">
         <f>IF(A45="","","Previsto")</f>
@@ -8027,7 +8032,7 @@
       </c>
       <c r="Q46" s="54">
         <f>IF(F46="","",ROUND((L46-G46)*SLA_ICP_EOS,1))</f>
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="R46" s="21">
         <f>IF(F46="","",SLA_ICP_CIHA)</f>
@@ -8063,7 +8068,7 @@
       </c>
       <c r="Z46" s="54">
         <f>IF(F46="","",ROUND((L46-G46)*SLA_ICA_EOS,1))</f>
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="AA46" t="str">
         <f>IF(A45="","","Homologação")</f>
@@ -8228,7 +8233,7 @@
       </c>
       <c r="L48" s="65">
         <f>IF(G46="","",ROUND((IF(P47="",P46,P47)/(19*LN(IF(P47="",P46,P47))-42))*30,0)+IF(VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="O48" s="27" t="str">
         <f>IF(A45="","","Multa")</f>
@@ -8322,7 +8327,7 @@
       </c>
       <c r="L49" s="65">
         <f>IF(G46="","",IF(IFERROR(VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A45,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="M49" s="20"/>
       <c r="N49" s="20"/>
@@ -8334,18 +8339,18 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4813</v>
       </c>
-      <c r="B50" s="113" t="str">
+      <c r="B50" s="114" t="str">
         <f>IF(A50="","",VLOOKUP(A50,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Plano Entregue</v>
       </c>
-      <c r="C50" s="113"/>
+      <c r="C50" s="114"/>
       <c r="D50" s="52" t="str">
         <f>IF(A50="","","em")</f>
         <v>em</v>
       </c>
       <c r="E50" s="56">
         <f>IF(A50="","",VLOOKUP(A50,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42633</v>
+        <v>42647</v>
       </c>
       <c r="F50" s="112" t="str">
         <f>IF(A50="","","Titulo:")</f>
@@ -8757,11 +8762,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B55" s="113" t="str">
+      <c r="B55" s="114" t="str">
         <f>IF(A55="","",VLOOKUP(A55,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C55" s="113"/>
+      <c r="C55" s="114"/>
       <c r="D55" s="52" t="str">
         <f>IF(A55="","","em")</f>
         <v/>
@@ -9180,11 +9185,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B60" s="113" t="str">
+      <c r="B60" s="114" t="str">
         <f>IF(A60="","",VLOOKUP(A60,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C60" s="113"/>
+      <c r="C60" s="114"/>
       <c r="D60" s="52" t="str">
         <f>IF(A60="","","em")</f>
         <v/>
@@ -9603,11 +9608,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B65" s="113" t="str">
+      <c r="B65" s="114" t="str">
         <f>IF(A65="","",VLOOKUP(A65,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C65" s="113"/>
+      <c r="C65" s="114"/>
       <c r="D65" s="52" t="str">
         <f>IF(A65="","","em")</f>
         <v/>
@@ -10026,11 +10031,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B70" s="113" t="str">
+      <c r="B70" s="114" t="str">
         <f>IF(A70="","",VLOOKUP(A70,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C70" s="113"/>
+      <c r="C70" s="114"/>
       <c r="D70" s="52" t="str">
         <f>IF(A70="","","em")</f>
         <v/>
@@ -10449,11 +10454,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B75" s="113" t="str">
+      <c r="B75" s="114" t="str">
         <f>IF(A75="","",VLOOKUP(A75,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C75" s="113"/>
+      <c r="C75" s="114"/>
       <c r="D75" s="52" t="str">
         <f>IF(A75="","","em")</f>
         <v/>
@@ -10872,11 +10877,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B80" s="113" t="str">
+      <c r="B80" s="114" t="str">
         <f>IF(A80="","",VLOOKUP(A80,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C80" s="113"/>
+      <c r="C80" s="114"/>
       <c r="D80" s="52" t="str">
         <f>IF(A80="","","em")</f>
         <v/>
@@ -11295,11 +11300,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B85" s="113" t="str">
+      <c r="B85" s="114" t="str">
         <f>IF(A85="","",VLOOKUP(A85,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C85" s="113"/>
+      <c r="C85" s="114"/>
       <c r="D85" s="52" t="str">
         <f>IF(A85="","","em")</f>
         <v/>
@@ -11718,11 +11723,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B90" s="113" t="str">
+      <c r="B90" s="114" t="str">
         <f>IF(A90="","",VLOOKUP(A90,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C90" s="113"/>
+      <c r="C90" s="114"/>
       <c r="D90" s="52" t="str">
         <f>IF(A90="","","em")</f>
         <v/>
@@ -12141,11 +12146,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B95" s="113" t="str">
+      <c r="B95" s="114" t="str">
         <f>IF(A95="","",VLOOKUP(A95,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C95" s="113"/>
+      <c r="C95" s="114"/>
       <c r="D95" s="52" t="str">
         <f>IF(A95="","","em")</f>
         <v/>
@@ -12564,11 +12569,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B100" s="113" t="str">
+      <c r="B100" s="114" t="str">
         <f>IF(A100="","",VLOOKUP(A100,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C100" s="113"/>
+      <c r="C100" s="114"/>
       <c r="D100" s="52" t="str">
         <f>IF(A100="","","em")</f>
         <v/>
@@ -12987,11 +12992,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B105" s="113" t="str">
+      <c r="B105" s="114" t="str">
         <f>IF(A105="","",VLOOKUP(A105,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C105" s="113"/>
+      <c r="C105" s="114"/>
       <c r="D105" s="52" t="str">
         <f>IF(A105="","","em")</f>
         <v/>
@@ -13410,11 +13415,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B110" s="113" t="str">
+      <c r="B110" s="114" t="str">
         <f>IF(A110="","",VLOOKUP(A110,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C110" s="113"/>
+      <c r="C110" s="114"/>
       <c r="D110" s="52" t="str">
         <f>IF(A110="","","em")</f>
         <v/>
@@ -13833,11 +13838,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B115" s="113" t="str">
+      <c r="B115" s="114" t="str">
         <f>IF(A115="","",VLOOKUP(A115,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C115" s="113"/>
+      <c r="C115" s="114"/>
       <c r="D115" s="52" t="str">
         <f>IF(A115="","","em")</f>
         <v/>
@@ -14256,11 +14261,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B120" s="113" t="str">
+      <c r="B120" s="114" t="str">
         <f>IF(A120="","",VLOOKUP(A120,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C120" s="113"/>
+      <c r="C120" s="114"/>
       <c r="D120" s="52" t="str">
         <f>IF(A120="","","em")</f>
         <v/>
@@ -14679,11 +14684,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B125" s="113" t="str">
+      <c r="B125" s="114" t="str">
         <f>IF(A125="","",VLOOKUP(A125,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C125" s="113"/>
+      <c r="C125" s="114"/>
       <c r="D125" s="52" t="str">
         <f>IF(A125="","","em")</f>
         <v/>
@@ -15102,11 +15107,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B130" s="113" t="str">
+      <c r="B130" s="114" t="str">
         <f>IF(A130="","",VLOOKUP(A130,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C130" s="113"/>
+      <c r="C130" s="114"/>
       <c r="D130" s="52" t="str">
         <f>IF(A130="","","em")</f>
         <v/>
@@ -15525,11 +15530,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B135" s="113" t="str">
+      <c r="B135" s="114" t="str">
         <f>IF(A135="","",VLOOKUP(A135,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C135" s="113"/>
+      <c r="C135" s="114"/>
       <c r="D135" s="52" t="str">
         <f>IF(A135="","","em")</f>
         <v/>
@@ -15948,11 +15953,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B140" s="113" t="str">
+      <c r="B140" s="114" t="str">
         <f>IF(A140="","",VLOOKUP(A140,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C140" s="113"/>
+      <c r="C140" s="114"/>
       <c r="D140" s="52" t="str">
         <f>IF(A140="","","em")</f>
         <v/>
@@ -16371,11 +16376,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B145" s="113" t="str">
+      <c r="B145" s="114" t="str">
         <f>IF(A145="","",VLOOKUP(A145,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C145" s="113"/>
+      <c r="C145" s="114"/>
       <c r="D145" s="52" t="str">
         <f>IF(A145="","","em")</f>
         <v/>
@@ -16794,11 +16799,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B150" s="113" t="str">
+      <c r="B150" s="114" t="str">
         <f>IF(A150="","",VLOOKUP(A150,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C150" s="113"/>
+      <c r="C150" s="114"/>
       <c r="D150" s="52" t="str">
         <f>IF(A150="","","em")</f>
         <v/>
@@ -17214,37 +17219,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B120:C120"/>
     <mergeCell ref="B150:C150"/>
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="B130:C130"/>
     <mergeCell ref="B135:C135"/>
     <mergeCell ref="B140:C140"/>
     <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -17261,7 +17266,7 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -17276,7 +17281,7 @@
         <v>203</v>
       </c>
       <c r="B1" s="21">
-        <v>4808</v>
+        <v>4809</v>
       </c>
       <c r="E1" t="s">
         <v>205</v>
@@ -17285,20 +17290,20 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <f>IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("Abertura da OS",OSS[#Headers],0),FALSE))</f>
-        <v>42590</v>
+        <v>42591</v>
       </c>
       <c r="B2" t="s">
         <v>108</v>
       </c>
       <c r="E2" s="109" t="str">
         <f>TEXT(A2,"DD/MM/AA")&amp;" "&amp;B2&amp;IF(C2="",""," "&amp;TEXT(C2,"DD/MM/AA"))</f>
-        <v>08/08/16 Abertura</v>
+        <v>09/08/16 Abertura</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <f>IF(A2="","",WORKDAY(A2,IF(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE))))&lt;150,5,10)))</f>
-        <v>42597</v>
+        <v>42605</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
@@ -17309,30 +17314,30 @@
       </c>
       <c r="E3" s="109" t="str">
         <f t="shared" ref="E3:E10" si="0">TEXT(A3,"DD/MM/AA")&amp;" "&amp;B3&amp;IF(C3="",""," "&amp;TEXT(C3,"DD/MM/AA"))</f>
-        <v>15/08/16 Inicio 15/08/16</v>
+        <v>23/08/16 Inicio 15/08/16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>IF(A3="","",WORKDAY(A3,5))</f>
-        <v>42604</v>
+        <v>42612</v>
       </c>
       <c r="B4" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="20" t="str">
         <f>IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
-        <v>42604</v>
+        <v/>
       </c>
       <c r="E4" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>22/08/16 Entrega do Plano 22/08/16</v>
+        <v>30/08/16 Entrega do Plano</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f>IF(A3="","",A3+ROUND((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))))-42))*30*SLA_PrazoEntrega,0)+IF(VLOOKUP(B1,OSS[#Data],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[#Data],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>42672</v>
+        <v>42726</v>
       </c>
       <c r="B5" t="s">
         <v>105</v>
@@ -17340,13 +17345,13 @@
       <c r="C5" s="20"/>
       <c r="E5" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>29/10/16 Entrega</v>
+        <v>22/12/16 Entrega</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f>IF(A5="","",WORKDAY(IF(C5="",A5,C5),IF(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE))))&lt;150,5,10)))</f>
-        <v>42678</v>
+        <v>42740</v>
       </c>
       <c r="B6" t="s">
         <v>206</v>
@@ -17354,13 +17359,13 @@
       <c r="C6" s="20"/>
       <c r="E6" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>04/11/16 Recebimento</v>
+        <v>05/01/17 Recebimento</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <f>IF(A6="","",A6+ROUND((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42689</v>
+        <v>42762</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -17371,13 +17376,13 @@
       </c>
       <c r="E7" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>15/11/16 Aceite</v>
+        <v>27/01/17 Aceite</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <f>IF(A3="","",A3+ROUND((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))))-42))*30,0)+IF(VLOOKUP(B1,OSS[#Data],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[#Data],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>42693</v>
+        <v>42770</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
@@ -17388,13 +17393,13 @@
       </c>
       <c r="E8" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>19/11/16 Termino</v>
+        <v>04/02/17 Termino</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <f>IF(A7="","",WORKDAY(A7,1))</f>
-        <v>42690</v>
+        <v>42765</v>
       </c>
       <c r="B9" t="s">
         <v>58</v>
@@ -17405,13 +17410,13 @@
       </c>
       <c r="E9" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>16/11/16 Garantia</v>
+        <v>30/01/17 Garantia</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f>IF(A9="","",A9+SLA_PrazoGarantia)</f>
-        <v>42870</v>
+        <v>42945</v>
       </c>
       <c r="B10" t="s">
         <v>107</v>
@@ -17422,7 +17427,7 @@
       </c>
       <c r="E10" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>15/05/17 Fim da Garantia</v>
+        <v>29/07/17 Fim da Garantia</v>
       </c>
     </row>
   </sheetData>
@@ -19112,11 +19117,11 @@
       </c>
       <c r="F1" s="20">
         <f ca="1">IF($G$1="",TODAY(),$G$1)</f>
-        <v>42648</v>
+        <v>42658</v>
       </c>
       <c r="G1" s="50">
         <f>IF(Mensal!B1="","",Mensal!B1)</f>
-        <v>42648</v>
+        <v>42658</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -19165,7 +19170,7 @@
       </c>
       <c r="F3" s="50">
         <f>IF(C3="","",VLOOKUP(C3,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42628</v>
+        <v>42636</v>
       </c>
       <c r="G3" s="21">
         <f t="shared" ref="G3:G16" si="1">IF(B3="",G2,IF(G2="",1,G2)+1)</f>
@@ -19195,7 +19200,7 @@
       </c>
       <c r="F4" s="50">
         <f>IF(C4="","",VLOOKUP(C4,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42639</v>
+        <v>42644</v>
       </c>
       <c r="G4" s="21">
         <f t="shared" si="1"/>
@@ -19225,7 +19230,7 @@
       </c>
       <c r="F5" s="50">
         <f>IF(C5="","",VLOOKUP(C5,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42628</v>
+        <v>42658</v>
       </c>
       <c r="G5" s="21">
         <f t="shared" si="1"/>
@@ -19256,7 +19261,7 @@
       </c>
       <c r="F6" s="50">
         <f>IF(C6="","",VLOOKUP(C6,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42647</v>
+        <v>42656</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="1"/>
@@ -19287,7 +19292,7 @@
       </c>
       <c r="F7" s="50">
         <f>IF(C7="","",VLOOKUP(C7,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42628</v>
+        <v>42660</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" si="1"/>
@@ -19411,7 +19416,7 @@
       </c>
       <c r="F11" s="50">
         <f>IF(C11="","",VLOOKUP(C11,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42639</v>
+        <v>42646</v>
       </c>
       <c r="G11" s="21">
         <f t="shared" si="1"/>
@@ -19442,7 +19447,7 @@
       </c>
       <c r="F12" s="50">
         <f>IF(C12="","",VLOOKUP(C12,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42633</v>
+        <v>42647</v>
       </c>
       <c r="G12" s="21">
         <f t="shared" si="1"/>

</xml_diff>